<commit_message>
testing logger+sync+extent report commit
</commit_message>
<xml_diff>
--- a/javaseleniumproject/src/test/resources/RegisterData.xlsx
+++ b/javaseleniumproject/src/test/resources/RegisterData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08B5D61-B9A1-47C4-81E6-BBBE7132DDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67BC177-85E6-45D4-B348-E6EA29EB9FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>FirstName</t>
   </si>
@@ -132,6 +132,27 @@
   </si>
   <si>
     <t>abhas@123</t>
+  </si>
+  <si>
+    <t>Bhagya</t>
+  </si>
+  <si>
+    <t>Shri</t>
+  </si>
+  <si>
+    <t>Nehru Nagar</t>
+  </si>
+  <si>
+    <t>Nashik</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>Bhagya3</t>
+  </si>
+  <si>
+    <t>bhagya@123</t>
   </si>
 </sst>
 </file>
@@ -503,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,8 +665,40 @@
       <c r="I4" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5">
+        <v>122333</v>
+      </c>
+      <c r="G5">
+        <v>7894561237</v>
+      </c>
+      <c r="H5">
+        <v>457891231</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -655,10 +708,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,6 +752,14 @@
         <v>36</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test Page Object Model Commit
</commit_message>
<xml_diff>
--- a/javaseleniumproject/src/test/resources/RegisterData.xlsx
+++ b/javaseleniumproject/src/test/resources/RegisterData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67BC177-85E6-45D4-B348-E6EA29EB9FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF49DC54-CFA5-4471-BD72-1D88F9A2BE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,12 +53,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Sai</t>
-  </si>
-  <si>
-    <t>Prabal</t>
-  </si>
-  <si>
     <t>Mallavarapu</t>
   </si>
   <si>
@@ -107,15 +101,6 @@
     <t>prabal@123</t>
   </si>
   <si>
-    <t>SaiSundar10</t>
-  </si>
-  <si>
-    <t>Ghosh10</t>
-  </si>
-  <si>
-    <t>Abhas</t>
-  </si>
-  <si>
     <t>Mittal</t>
   </si>
   <si>
@@ -128,15 +113,9 @@
     <t>UP</t>
   </si>
   <si>
-    <t>Abhas1</t>
-  </si>
-  <si>
     <t>abhas@123</t>
   </si>
   <si>
-    <t>Bhagya</t>
-  </si>
-  <si>
     <t>Shri</t>
   </si>
   <si>
@@ -149,10 +128,31 @@
     <t>MH</t>
   </si>
   <si>
-    <t>Bhagya3</t>
-  </si>
-  <si>
     <t>bhagya@123</t>
+  </si>
+  <si>
+    <t>Sai1</t>
+  </si>
+  <si>
+    <t>Prabal2</t>
+  </si>
+  <si>
+    <t>Abhas3</t>
+  </si>
+  <si>
+    <t>Bhagya4</t>
+  </si>
+  <si>
+    <t>SaiSundar101</t>
+  </si>
+  <si>
+    <t>Ghosh102</t>
+  </si>
+  <si>
+    <t>Abhas103</t>
+  </si>
+  <si>
+    <t>Bhagya104</t>
   </si>
 </sst>
 </file>
@@ -211,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -219,7 +219,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,7 +526,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,83 +574,83 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
         <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
         <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F4">
         <v>250004</v>
@@ -663,27 +662,27 @@
         <v>159753462</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F5">
         <v>122333</v>
@@ -695,10 +694,10 @@
         <v>457891231</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="3" t="s">
         <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -711,7 +710,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,34 +729,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="3" t="s">
         <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>